<commit_message>
Finalização do tópico 5.
</commit_message>
<xml_diff>
--- a/Banco_de_Dados_Relacional/5.08.insercao-dados-dp.db/dados/ResponsavelDP.xlsx
+++ b/Banco_de_Dados_Relacional/5.08.insercao-dados-dp.db/dados/ResponsavelDP.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27321"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4a4df0780b30e7fd/Claudio Bonel-DADOTECA/_ProfessorClaudioBonel/PUCRS/Banco de dados relacional/Dados/Exercício/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{15F77C6C-8C2C-49A5-B862-3B741DFCFC89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8D24E65A-3474-4714-933B-76DEBE0311E1}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2CC68E54-FC43-4715-A381-9C9C82420F44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,432 +16,448 @@
     <sheet name="ResponsavelDP" sheetId="1" r:id="rId1"/>
     <sheet name="respDP_old" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="138">
   <si>
+    <t>codigo_dp</t>
+  </si>
+  <si>
+    <t>delegado</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia José Luiz Silva Duarte</t>
+  </si>
+  <si>
+    <t>Delegada de Polícia Patricia de Paiva Aguiar</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Bruno Gilaberte Freitas</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Fabio Luiz Da Silva Souza</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Carlos Alberto Meirelles De Abreu Filho</t>
+  </si>
+  <si>
+    <t>Delegada de Polícia Maria Aparecida Salgado Mallet</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Alexandre Herdy Barros Silva</t>
+  </si>
+  <si>
+    <t>Delegada de Polícia Flávia Goes Monteiro Romero de Barros</t>
+  </si>
+  <si>
+    <t>Delegada de Polícia Bianca Rodrigues Xavier Lima de Vasconcelos</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Felipe Santoro da Silva</t>
+  </si>
+  <si>
+    <t>Delegada de Polícia Natacha Alves de Oliveira</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Daniel Freitas da Rosa</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Leandro Gontijo de Siqueira Alves</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Marcio Esteves de Jesus</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Moysés Santana Gomes</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Gabriel Ferrando de Almeida</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Cristiano do Vale Maia</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Hilton Pinho Alonso</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Wellington Pereira Vieira</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Deoclecio Francisco de Assis Filho</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Tiago Venturini Antunes</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Renato dos Santos Mariano</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia João Luiz Garcia de Almeida e Costa</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Renato Bezerra Carvalho</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Victor Arthur Tuttman Diegues</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Neilson dos Santos Nogueira</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Rodolfo Waldeck Penco Monteiro</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Marcio Petra de Mello</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Alessandro Petralanda Santos</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Rodrigo de Barros Piedras Lopes</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Luis Mauricio Armond Campos</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Túlio Antônio Pelosi</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Adilson Palácio</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Marcus Henrique de Oliveira Alves</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Mauricio Mendonça de Carvalho</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Thiago Dorigo</t>
+  </si>
+  <si>
+    <t>Delegada de Polícia Márcia Beck Simões</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Reginaldo Guilherme da Silva</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Alan Luxardo</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Antonio Ricardo Lima Nunes</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Alexandre Henrique Duarte Braga</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Reginaldo Felix Vall Lloveras</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Marco Aurelio Castro</t>
+  </si>
+  <si>
+    <t>Delegada de Polícia Rita de Cassia Salim Tavares</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Celso Gustavo Castello Ribeiro</t>
+  </si>
+  <si>
+    <t>Delegada de Polícia Juliana Emerique de Amorim Coutinho</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia José Mário Salomão de Omena</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Bruno Enrique de Abreu Menezes</t>
+  </si>
+  <si>
+    <t>Delegada de Polícia Bárbara Lomba Bueno</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia José de Moraes Ferreira</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Willians Batista de Souza</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Andre Barbosa Morais</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Paulo Roberto Lima de Freitas</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Roberto Gomes Nunes</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Marcos Santana Gomes</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Flávio Ferreira Rodrigues</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Evaristo Pontes Magalhães</t>
+  </si>
+  <si>
+    <t>Delegada de Polícia Isabelle Conti de Almeida</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Angelo José Lages Machado</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Antonio Silvino Teixeira</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Mário Luiz da Silva</t>
+  </si>
+  <si>
+    <t>Delegada de Polícia Norma Passos Lacerda de Oliveira</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Allan Duarte Lacerda</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Leonardo Luis Macharet</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Lauro Cesar Lethier Rangel</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Cláudio Vieira de Campos</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Luis Henrique Marques Pereira</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Claudio Otero Ascioli</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Geraldo Assed Estefan</t>
+  </si>
+  <si>
+    <t>Delegada de Polícia Raissa Maria dos Santos Celles</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Fábio Oliveira Barucke</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Luiz Henrique Ferreira Guimarães</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Rodolfo Bonfante Atala</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Michel Andre Murillo Floroschk</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Ronaldo Aparecido Ferreira Brito</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Carlos Cesar Santos</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Edezio de Castro Ramos Junior</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Carlos Henrique Pereira Machado</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Jorge Rodrigues da Silva</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia André Luiz Alves Uchoa</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia João Ricardo Bicudo de Oliveira</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Luiz Fernando Nader Damasceno</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Vicente Maximiliano Rodrigues Barbosa</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Marcelo Nunes Ribeiro</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Fabio Asty Dantas</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Paulo César Vieira</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia João Valentim dos Santos Neto</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Nei José Ramos Loureiro</t>
+  </si>
+  <si>
+    <t>Delegada de Polícia Claudia Teresa Nardy Abbud</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Claudio Batista Teixeira</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia André Luiz Pinto Lourenço</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Marcio Mendonça Dubugras</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Vinícius Paiva Galhardo</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Herbert Tavares Cardoso</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Filipi Poeys Lima</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Aloysio Berardo Falcão de Paula Lopes</t>
+  </si>
+  <si>
+    <t>Delegada de Polícia Janaina Cristina Peregrino</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Ivailson Moreira Sardinha</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Sérgio Elias Santana Junior</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Márcio Caldas Dias Mello</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Andre Luiz Salvador Bueno</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Milton Siqueira Junior</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Carlos Eduardo Pereira Almeida</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Rodrigo Bichara Moreira</t>
+  </si>
+  <si>
+    <t>Delegada de Polícia Roberto Ramos da Silva</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Fabio Corsino Freire</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Raul Gustavo Morgado</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Ruchester Marreiros Barbosa</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Ronaldo Andrade Cavalcante</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Rodrigo Vinícius Andrade Maia</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Mário César Monerat Vianna</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Gesner Cesar Bruno</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Gesner César Bruno</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Uillian Rodrigues da Costa</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Carlos Augusto G. da Silva</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Avelino da Costa Lima Filho</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Henrique Vitor Lobato</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Jorge Luiz da Silva Veloso</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Rodolfo Maravilha Franco da Silva</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Pedro Emílio de Souza Braga</t>
+  </si>
+  <si>
+    <t>Delegada de Polícia Ivana Maria Peres Morgado</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Rivelino Da Silva Bueno</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Henrique Paulo Mesquita Pessôa</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Diogo Teixeira Schettini</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Robson Pizzo Braga</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Gilberto Soares da Silva</t>
+  </si>
+  <si>
+    <t>Delegada de Polícia Carla Vargas de Oliveira</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Franquis Dias Nepomuceno</t>
+  </si>
+  <si>
+    <t>Delegada de Polícia Danielle Christine Bessa Neto de Barros</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Clovis Souza Moreira</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Anderson Ribeiro Pinto</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Vilson de Almeida Silva</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Marcelo dos Santos Haddad</t>
+  </si>
+  <si>
+    <t>Delegado de Polícia Francisco Benitez Lopes</t>
+  </si>
+  <si>
     <t>COD_DP</t>
   </si>
   <si>
     <t>Responsavel</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia José Luiz Silva Duarte</t>
-  </si>
-  <si>
-    <t>Delegada de Polícia Patricia de Paiva Aguiar</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Bruno Gilaberte Freitas</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Fabio Luiz Da Silva Souza</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Carlos Alberto Meirelles De Abreu Filho</t>
-  </si>
-  <si>
-    <t>Delegada de Polícia Maria Aparecida Salgado Mallet</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Alexandre Herdy Barros Silva</t>
-  </si>
-  <si>
-    <t>Delegada de Polícia Flávia Goes Monteiro Romero de Barros</t>
-  </si>
-  <si>
-    <t>Delegada de Polícia Bianca Rodrigues Xavier Lima de Vasconcelos</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Felipe Santoro da Silva</t>
-  </si>
-  <si>
-    <t>Delegada de Polícia Natacha Alves de Oliveira</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Daniel Freitas da Rosa</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Leandro Gontijo de Siqueira Alves</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Marcio Esteves de Jesus</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Moysés Santana Gomes</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Gabriel Ferrando de Almeida</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Cristiano do Vale Maia</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Hilton Pinho Alonso</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Wellington Pereira Vieira</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Deoclecio Francisco de Assis Filho</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Tiago Venturini Antunes</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Renato dos Santos Mariano</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia João Luiz Garcia de Almeida e Costa</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Renato Bezerra Carvalho</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Victor Arthur Tuttman Diegues</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Neilson dos Santos Nogueira</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Rodolfo Waldeck Penco Monteiro</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Marcio Petra de Mello</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Alessandro Petralanda Santos</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Rodrigo de Barros Piedras Lopes</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Luis Mauricio Armond Campos</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Túlio Antônio Pelosi</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Adilson Palácio</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Marcus Henrique de Oliveira Alves</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Mauricio Mendonça de Carvalho</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Thiago Dorigo</t>
-  </si>
-  <si>
-    <t>Delegada de Polícia Márcia Beck Simões</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Reginaldo Guilherme da Silva</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Alan Luxardo</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Antonio Ricardo Lima Nunes</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Alexandre Henrique Duarte Braga</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Reginaldo Felix Vall Lloveras</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Marco Aurelio Castro</t>
-  </si>
-  <si>
-    <t>Delegada de Polícia Rita de Cassia Salim Tavares</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Celso Gustavo Castello Ribeiro</t>
-  </si>
-  <si>
-    <t>Delegada de Polícia Juliana Emerique de Amorim Coutinho</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia José Mário Salomão de Omena</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Bruno Enrique de Abreu Menezes</t>
-  </si>
-  <si>
-    <t>Delegada de Polícia Bárbara Lomba Bueno</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia José de Moraes Ferreira</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Willians Batista de Souza</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Andre Barbosa Morais</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Paulo Roberto Lima de Freitas</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Roberto Gomes Nunes</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Marcos Santana Gomes</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Flávio Ferreira Rodrigues</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Evaristo Pontes Magalhães</t>
-  </si>
-  <si>
-    <t>Delegada de Polícia Isabelle Conti de Almeida</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Angelo José Lages Machado</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Antonio Silvino Teixeira</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Mário Luiz da Silva</t>
-  </si>
-  <si>
-    <t>Delegada de Polícia Norma Passos Lacerda de Oliveira</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Allan Duarte Lacerda</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Leonardo Luis Macharet</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Lauro Cesar Lethier Rangel</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Cláudio Vieira de Campos</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Luis Henrique Marques Pereira</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Claudio Otero Ascioli</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Geraldo Assed Estefan</t>
-  </si>
-  <si>
-    <t>Delegada de Polícia Raissa Maria dos Santos Celles</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Fábio Oliveira Barucke</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Luiz Henrique Ferreira Guimarães</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Rodolfo Bonfante Atala</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Michel Andre Murillo Floroschk</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Ronaldo Aparecido Ferreira Brito</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Carlos Cesar Santos</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Edezio de Castro Ramos Junior</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Carlos Henrique Pereira Machado</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Jorge Rodrigues da Silva</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia André Luiz Alves Uchoa</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia João Ricardo Bicudo de Oliveira</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Luiz Fernando Nader Damasceno</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Vicente Maximiliano Rodrigues Barbosa</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Marcelo Nunes Ribeiro</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Fabio Asty Dantas</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Paulo César Vieira</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia João Valentim dos Santos Neto</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Nei José Ramos Loureiro</t>
-  </si>
-  <si>
-    <t>Delegada de Polícia Claudia Teresa Nardy Abbud</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Claudio Batista Teixeira</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia André Luiz Pinto Lourenço</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Marcio Mendonça Dubugras</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Vinícius Paiva Galhardo</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Herbert Tavares Cardoso</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Filipi Poeys Lima</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Aloysio Berardo Falcão de Paula Lopes</t>
-  </si>
-  <si>
-    <t>Delegada de Polícia Janaina Cristina Peregrino</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Ivailson Moreira Sardinha</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Sérgio Elias Santana Junior</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Márcio Caldas Dias Mello</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Andre Luiz Salvador Bueno</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Milton Siqueira Junior</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Carlos Eduardo Pereira Almeida</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Rodrigo Bichara Moreira</t>
-  </si>
-  <si>
-    <t>Delegada de Polícia Roberto Ramos da Silva</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Fabio Corsino Freire</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Raul Gustavo Morgado</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Ruchester Marreiros Barbosa</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Ronaldo Andrade Cavalcante</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Rodrigo Vinícius Andrade Maia</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Mário César Monerat Vianna</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Gesner Cesar Bruno</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Gesner César Bruno</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Uillian Rodrigues da Costa</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Carlos Augusto G. da Silva</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Avelino da Costa Lima Filho</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Henrique Vitor Lobato</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Jorge Luiz da Silva Veloso</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Rodolfo Maravilha Franco da Silva</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Pedro Emílio de Souza Braga</t>
-  </si>
-  <si>
-    <t>Delegada de Polícia Ivana Maria Peres Morgado</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Rivelino Da Silva Bueno</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Henrique Paulo Mesquita Pessôa</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Diogo Teixeira Schettini</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Robson Pizzo Braga</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Gilberto Soares da Silva</t>
-  </si>
-  <si>
-    <t>Delegada de Polícia Carla Vargas de Oliveira</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Franquis Dias Nepomuceno</t>
-  </si>
-  <si>
-    <t>Delegada de Polícia Danielle Christine Bessa Neto de Barros</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Clovis Souza Moreira</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Anderson Ribeiro Pinto</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Vilson de Almeida Silva</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Marcelo dos Santos Haddad</t>
-  </si>
-  <si>
-    <t>Delegado de Polícia Francisco Benitez Lopes</t>
-  </si>
-  <si>
-    <t>codDP</t>
-  </si>
-  <si>
-    <t>delegado</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -979,7 +995,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1277,21 +1293,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B138"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>136</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1299,7 +1313,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>4</v>
       </c>
@@ -1307,7 +1321,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2">
       <c r="A4">
         <v>5</v>
       </c>
@@ -1315,7 +1329,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2">
       <c r="A5">
         <v>6</v>
       </c>
@@ -1323,7 +1337,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2">
       <c r="A6">
         <v>7</v>
       </c>
@@ -1331,7 +1345,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2">
       <c r="A7">
         <v>9</v>
       </c>
@@ -1339,7 +1353,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2">
       <c r="A8">
         <v>10</v>
       </c>
@@ -1347,7 +1361,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2">
       <c r="A9">
         <v>11</v>
       </c>
@@ -1355,7 +1369,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2">
       <c r="A10">
         <v>12</v>
       </c>
@@ -1363,7 +1377,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2">
       <c r="A11">
         <v>13</v>
       </c>
@@ -1371,7 +1385,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2">
       <c r="A12">
         <v>14</v>
       </c>
@@ -1379,7 +1393,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2">
       <c r="A13">
         <v>15</v>
       </c>
@@ -1387,7 +1401,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2">
       <c r="A14">
         <v>16</v>
       </c>
@@ -1395,7 +1409,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2">
       <c r="A15">
         <v>17</v>
       </c>
@@ -1403,7 +1417,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2">
       <c r="A16">
         <v>18</v>
       </c>
@@ -1411,7 +1425,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2">
       <c r="A17">
         <v>19</v>
       </c>
@@ -1419,7 +1433,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2">
       <c r="A18">
         <v>20</v>
       </c>
@@ -1427,7 +1441,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2">
       <c r="A19">
         <v>21</v>
       </c>
@@ -1435,7 +1449,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2">
       <c r="A20">
         <v>22</v>
       </c>
@@ -1443,7 +1457,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2">
       <c r="A21">
         <v>23</v>
       </c>
@@ -1451,7 +1465,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2">
       <c r="A22">
         <v>24</v>
       </c>
@@ -1459,7 +1473,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2">
       <c r="A23">
         <v>25</v>
       </c>
@@ -1467,7 +1481,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2">
       <c r="A24">
         <v>26</v>
       </c>
@@ -1475,7 +1489,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2">
       <c r="A25">
         <v>27</v>
       </c>
@@ -1483,7 +1497,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2">
       <c r="A26">
         <v>28</v>
       </c>
@@ -1491,7 +1505,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2">
       <c r="A27">
         <v>29</v>
       </c>
@@ -1499,7 +1513,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2">
       <c r="A28">
         <v>30</v>
       </c>
@@ -1507,7 +1521,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2">
       <c r="A29">
         <v>31</v>
       </c>
@@ -1515,7 +1529,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2">
       <c r="A30">
         <v>32</v>
       </c>
@@ -1523,7 +1537,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2">
       <c r="A31">
         <v>33</v>
       </c>
@@ -1531,7 +1545,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2">
       <c r="A32">
         <v>34</v>
       </c>
@@ -1539,7 +1553,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2">
       <c r="A33">
         <v>35</v>
       </c>
@@ -1547,7 +1561,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2">
       <c r="A34">
         <v>36</v>
       </c>
@@ -1555,7 +1569,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2">
       <c r="A35">
         <v>37</v>
       </c>
@@ -1563,7 +1577,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2">
       <c r="A36">
         <v>38</v>
       </c>
@@ -1571,7 +1585,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2">
       <c r="A37">
         <v>39</v>
       </c>
@@ -1579,7 +1593,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2">
       <c r="A38">
         <v>40</v>
       </c>
@@ -1587,7 +1601,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2">
       <c r="A39">
         <v>41</v>
       </c>
@@ -1595,7 +1609,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2">
       <c r="A40">
         <v>42</v>
       </c>
@@ -1603,7 +1617,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2">
       <c r="A41">
         <v>43</v>
       </c>
@@ -1611,7 +1625,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2">
       <c r="A42">
         <v>44</v>
       </c>
@@ -1619,7 +1633,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2">
       <c r="A43">
         <v>48</v>
       </c>
@@ -1627,7 +1641,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2">
       <c r="A44">
         <v>50</v>
       </c>
@@ -1635,7 +1649,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2">
       <c r="A45">
         <v>51</v>
       </c>
@@ -1643,7 +1657,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2">
       <c r="A46">
         <v>52</v>
       </c>
@@ -1651,7 +1665,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2">
       <c r="A47">
         <v>53</v>
       </c>
@@ -1659,7 +1673,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2">
       <c r="A48">
         <v>54</v>
       </c>
@@ -1667,7 +1681,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2">
       <c r="A49">
         <v>55</v>
       </c>
@@ -1675,7 +1689,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2">
       <c r="A50">
         <v>56</v>
       </c>
@@ -1683,7 +1697,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2">
       <c r="A51">
         <v>57</v>
       </c>
@@ -1691,7 +1705,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2">
       <c r="A52">
         <v>58</v>
       </c>
@@ -1699,7 +1713,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2">
       <c r="A53">
         <v>59</v>
       </c>
@@ -1707,7 +1721,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2">
       <c r="A54">
         <v>60</v>
       </c>
@@ -1715,7 +1729,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2">
       <c r="A55">
         <v>61</v>
       </c>
@@ -1723,7 +1737,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2">
       <c r="A56">
         <v>62</v>
       </c>
@@ -1731,7 +1745,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2">
       <c r="A57">
         <v>63</v>
       </c>
@@ -1739,7 +1753,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2">
       <c r="A58">
         <v>64</v>
       </c>
@@ -1747,7 +1761,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2">
       <c r="A59">
         <v>65</v>
       </c>
@@ -1755,7 +1769,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2">
       <c r="A60">
         <v>66</v>
       </c>
@@ -1763,7 +1777,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2">
       <c r="A61">
         <v>67</v>
       </c>
@@ -1771,7 +1785,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2">
       <c r="A62">
         <v>70</v>
       </c>
@@ -1779,7 +1793,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2">
       <c r="A63">
         <v>71</v>
       </c>
@@ -1787,7 +1801,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2">
       <c r="A64">
         <v>72</v>
       </c>
@@ -1795,7 +1809,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2">
       <c r="A65">
         <v>73</v>
       </c>
@@ -1803,7 +1817,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2">
       <c r="A66">
         <v>74</v>
       </c>
@@ -1811,7 +1825,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2">
       <c r="A67">
         <v>75</v>
       </c>
@@ -1819,7 +1833,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2">
       <c r="A68">
         <v>76</v>
       </c>
@@ -1827,7 +1841,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2">
       <c r="A69">
         <v>77</v>
       </c>
@@ -1835,7 +1849,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2">
       <c r="A70">
         <v>78</v>
       </c>
@@ -1843,7 +1857,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2">
       <c r="A71">
         <v>79</v>
       </c>
@@ -1851,7 +1865,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2">
       <c r="A72">
         <v>81</v>
       </c>
@@ -1859,7 +1873,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2">
       <c r="A73">
         <v>82</v>
       </c>
@@ -1867,7 +1881,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2">
       <c r="A74">
         <v>88</v>
       </c>
@@ -1875,7 +1889,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2">
       <c r="A75">
         <v>89</v>
       </c>
@@ -1883,7 +1897,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2">
       <c r="A76">
         <v>90</v>
       </c>
@@ -1891,7 +1905,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:2">
       <c r="A77">
         <v>91</v>
       </c>
@@ -1899,7 +1913,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:2">
       <c r="A78">
         <v>92</v>
       </c>
@@ -1907,7 +1921,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:2">
       <c r="A79">
         <v>93</v>
       </c>
@@ -1915,7 +1929,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:2">
       <c r="A80">
         <v>94</v>
       </c>
@@ -1923,7 +1937,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2">
       <c r="A81">
         <v>95</v>
       </c>
@@ -1931,7 +1945,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:2">
       <c r="A82">
         <v>96</v>
       </c>
@@ -1939,7 +1953,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:2">
       <c r="A83">
         <v>97</v>
       </c>
@@ -1947,7 +1961,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:2">
       <c r="A84">
         <v>98</v>
       </c>
@@ -1955,7 +1969,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:2">
       <c r="A85">
         <v>99</v>
       </c>
@@ -1963,7 +1977,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:2">
       <c r="A86">
         <v>100</v>
       </c>
@@ -1971,7 +1985,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:2">
       <c r="A87">
         <v>101</v>
       </c>
@@ -1979,7 +1993,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:2">
       <c r="A88">
         <v>104</v>
       </c>
@@ -1987,7 +2001,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:2">
       <c r="A89">
         <v>105</v>
       </c>
@@ -1995,7 +2009,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:2">
       <c r="A90">
         <v>106</v>
       </c>
@@ -2003,7 +2017,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:2">
       <c r="A91">
         <v>107</v>
       </c>
@@ -2011,7 +2025,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:2">
       <c r="A92">
         <v>108</v>
       </c>
@@ -2019,7 +2033,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:2">
       <c r="A93">
         <v>109</v>
       </c>
@@ -2027,7 +2041,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:2">
       <c r="A94">
         <v>110</v>
       </c>
@@ -2035,7 +2049,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:2">
       <c r="A95">
         <v>111</v>
       </c>
@@ -2043,7 +2057,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:2">
       <c r="A96">
         <v>112</v>
       </c>
@@ -2051,7 +2065,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:2">
       <c r="A97">
         <v>118</v>
       </c>
@@ -2059,7 +2073,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:2">
       <c r="A98">
         <v>119</v>
       </c>
@@ -2067,7 +2081,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:2">
       <c r="A99">
         <v>120</v>
       </c>
@@ -2075,7 +2089,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:2">
       <c r="A100">
         <v>121</v>
       </c>
@@ -2083,7 +2097,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:2">
       <c r="A101">
         <v>122</v>
       </c>
@@ -2091,7 +2105,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:2">
       <c r="A102">
         <v>123</v>
       </c>
@@ -2099,7 +2113,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:2">
       <c r="A103">
         <v>124</v>
       </c>
@@ -2107,7 +2121,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:2">
       <c r="A104">
         <v>125</v>
       </c>
@@ -2115,7 +2129,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:2">
       <c r="A105">
         <v>126</v>
       </c>
@@ -2123,7 +2137,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:2">
       <c r="A106">
         <v>127</v>
       </c>
@@ -2131,7 +2145,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:2">
       <c r="A107">
         <v>128</v>
       </c>
@@ -2139,7 +2153,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:2">
       <c r="A108">
         <v>129</v>
       </c>
@@ -2147,7 +2161,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:2">
       <c r="A109">
         <v>130</v>
       </c>
@@ -2155,7 +2169,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:2">
       <c r="A110">
         <v>132</v>
       </c>
@@ -2163,7 +2177,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:2">
       <c r="A111">
         <v>134</v>
       </c>
@@ -2171,7 +2185,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:2">
       <c r="A112">
         <v>135</v>
       </c>
@@ -2179,7 +2193,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:2">
       <c r="A113">
         <v>136</v>
       </c>
@@ -2187,7 +2201,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:2">
       <c r="A114">
         <v>137</v>
       </c>
@@ -2195,7 +2209,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:2">
       <c r="A115">
         <v>138</v>
       </c>
@@ -2203,7 +2217,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:2">
       <c r="A116">
         <v>139</v>
       </c>
@@ -2211,7 +2225,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:2">
       <c r="A117">
         <v>140</v>
       </c>
@@ -2219,7 +2233,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:2">
       <c r="A118">
         <v>141</v>
       </c>
@@ -2227,7 +2241,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:2">
       <c r="A119">
         <v>142</v>
       </c>
@@ -2235,7 +2249,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:2">
       <c r="A120">
         <v>143</v>
       </c>
@@ -2243,7 +2257,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:2">
       <c r="A121">
         <v>144</v>
       </c>
@@ -2251,7 +2265,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:2">
       <c r="A122">
         <v>145</v>
       </c>
@@ -2259,7 +2273,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:2">
       <c r="A123">
         <v>146</v>
       </c>
@@ -2267,7 +2281,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:2">
       <c r="A124">
         <v>147</v>
       </c>
@@ -2275,7 +2289,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:2">
       <c r="A125">
         <v>148</v>
       </c>
@@ -2283,7 +2297,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:2">
       <c r="A126">
         <v>151</v>
       </c>
@@ -2291,7 +2305,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:2">
       <c r="A127">
         <v>152</v>
       </c>
@@ -2299,7 +2313,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:2">
       <c r="A128">
         <v>153</v>
       </c>
@@ -2307,7 +2321,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:2">
       <c r="A129">
         <v>154</v>
       </c>
@@ -2315,7 +2329,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:2">
       <c r="A130">
         <v>155</v>
       </c>
@@ -2323,7 +2337,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:2">
       <c r="A131">
         <v>156</v>
       </c>
@@ -2331,7 +2345,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:2">
       <c r="A132">
         <v>157</v>
       </c>
@@ -2339,7 +2353,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:2">
       <c r="A133">
         <v>158</v>
       </c>
@@ -2347,7 +2361,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:2">
       <c r="A134">
         <v>159</v>
       </c>
@@ -2355,7 +2369,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:2">
       <c r="A135">
         <v>165</v>
       </c>
@@ -2363,7 +2377,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:2">
       <c r="A136">
         <v>166</v>
       </c>
@@ -2371,7 +2385,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:2">
       <c r="A137">
         <v>167</v>
       </c>
@@ -2379,7 +2393,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:2">
       <c r="A138">
         <v>168</v>
       </c>
@@ -2400,17 +2414,17 @@
       <selection activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>136</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2418,7 +2432,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>4</v>
       </c>
@@ -2426,7 +2440,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2">
       <c r="A4">
         <v>5</v>
       </c>
@@ -2434,7 +2448,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2">
       <c r="A5">
         <v>6</v>
       </c>
@@ -2442,7 +2456,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2">
       <c r="A6">
         <v>7</v>
       </c>
@@ -2450,7 +2464,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2">
       <c r="A7">
         <v>9</v>
       </c>
@@ -2458,7 +2472,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2">
       <c r="A8">
         <v>10</v>
       </c>
@@ -2466,7 +2480,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2">
       <c r="A9">
         <v>11</v>
       </c>
@@ -2474,7 +2488,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2">
       <c r="A10">
         <v>12</v>
       </c>
@@ -2482,7 +2496,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2">
       <c r="A11">
         <v>13</v>
       </c>
@@ -2490,7 +2504,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2">
       <c r="A12">
         <v>14</v>
       </c>
@@ -2498,7 +2512,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2">
       <c r="A13">
         <v>15</v>
       </c>
@@ -2506,7 +2520,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2">
       <c r="A14">
         <v>16</v>
       </c>
@@ -2514,7 +2528,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2">
       <c r="A15">
         <v>17</v>
       </c>
@@ -2522,7 +2536,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2">
       <c r="A16">
         <v>18</v>
       </c>
@@ -2530,7 +2544,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2">
       <c r="A17">
         <v>19</v>
       </c>
@@ -2538,7 +2552,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2">
       <c r="A18">
         <v>20</v>
       </c>
@@ -2546,7 +2560,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2">
       <c r="A19">
         <v>21</v>
       </c>
@@ -2554,7 +2568,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2">
       <c r="A20">
         <v>22</v>
       </c>
@@ -2562,7 +2576,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2">
       <c r="A21">
         <v>23</v>
       </c>
@@ -2570,7 +2584,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2">
       <c r="A22">
         <v>24</v>
       </c>
@@ -2578,7 +2592,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2">
       <c r="A23">
         <v>25</v>
       </c>
@@ -2586,7 +2600,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2">
       <c r="A24">
         <v>26</v>
       </c>
@@ -2594,7 +2608,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2">
       <c r="A25">
         <v>27</v>
       </c>
@@ -2602,7 +2616,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2">
       <c r="A26">
         <v>28</v>
       </c>
@@ -2610,7 +2624,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2">
       <c r="A27">
         <v>29</v>
       </c>
@@ -2618,7 +2632,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2">
       <c r="A28">
         <v>30</v>
       </c>
@@ -2626,7 +2640,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2">
       <c r="A29">
         <v>31</v>
       </c>
@@ -2634,7 +2648,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2">
       <c r="A30">
         <v>32</v>
       </c>
@@ -2642,7 +2656,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2">
       <c r="A31">
         <v>33</v>
       </c>
@@ -2650,7 +2664,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2">
       <c r="A32">
         <v>34</v>
       </c>
@@ -2658,7 +2672,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2">
       <c r="A33">
         <v>35</v>
       </c>
@@ -2666,7 +2680,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2">
       <c r="A34">
         <v>36</v>
       </c>
@@ -2674,7 +2688,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2">
       <c r="A35">
         <v>37</v>
       </c>
@@ -2682,7 +2696,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2">
       <c r="A36">
         <v>38</v>
       </c>
@@ -2690,7 +2704,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2">
       <c r="A37">
         <v>39</v>
       </c>
@@ -2698,7 +2712,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2">
       <c r="A38">
         <v>40</v>
       </c>
@@ -2706,7 +2720,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2">
       <c r="A39">
         <v>79</v>
       </c>
@@ -2714,7 +2728,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2">
       <c r="A40">
         <v>81</v>
       </c>
@@ -2722,7 +2736,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2">
       <c r="A41">
         <v>82</v>
       </c>
@@ -2730,7 +2744,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2">
       <c r="A42">
         <v>88</v>
       </c>
@@ -2738,7 +2752,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2">
       <c r="A43">
         <v>89</v>
       </c>
@@ -2746,7 +2760,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2">
       <c r="A44">
         <v>90</v>
       </c>
@@ -2754,7 +2768,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2">
       <c r="A45">
         <v>91</v>
       </c>
@@ -2762,7 +2776,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2">
       <c r="A46">
         <v>92</v>
       </c>
@@ -2770,7 +2784,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2">
       <c r="A47">
         <v>93</v>
       </c>
@@ -2778,7 +2792,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2">
       <c r="A48">
         <v>94</v>
       </c>
@@ -2786,7 +2800,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2">
       <c r="A49">
         <v>95</v>
       </c>
@@ -2794,7 +2808,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2">
       <c r="A50">
         <v>96</v>
       </c>
@@ -2802,7 +2816,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2">
       <c r="A51">
         <v>97</v>
       </c>
@@ -2810,7 +2824,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2">
       <c r="A52">
         <v>98</v>
       </c>
@@ -2818,7 +2832,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2">
       <c r="A53">
         <v>99</v>
       </c>
@@ -2826,7 +2840,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2">
       <c r="A54">
         <v>100</v>
       </c>
@@ -2834,7 +2848,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2">
       <c r="A55">
         <v>101</v>
       </c>
@@ -2842,7 +2856,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2">
       <c r="A56">
         <v>104</v>
       </c>
@@ -2850,7 +2864,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2">
       <c r="A57">
         <v>105</v>
       </c>
@@ -2858,7 +2872,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2">
       <c r="A58">
         <v>106</v>
       </c>
@@ -2866,7 +2880,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2">
       <c r="A59">
         <v>107</v>
       </c>
@@ -2874,7 +2888,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2">
       <c r="A60">
         <v>108</v>
       </c>
@@ -2882,7 +2896,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2">
       <c r="A61">
         <v>109</v>
       </c>
@@ -2890,7 +2904,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2">
       <c r="A62">
         <v>110</v>
       </c>
@@ -2898,7 +2912,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2">
       <c r="A63">
         <v>111</v>
       </c>
@@ -2906,7 +2920,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2">
       <c r="A64">
         <v>112</v>
       </c>
@@ -2914,7 +2928,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2">
       <c r="A65">
         <v>118</v>
       </c>
@@ -2922,7 +2936,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2">
       <c r="A66">
         <v>119</v>
       </c>
@@ -2930,7 +2944,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2">
       <c r="A67">
         <v>120</v>
       </c>
@@ -2938,7 +2952,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2">
       <c r="A68">
         <v>121</v>
       </c>
@@ -2946,7 +2960,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2">
       <c r="A69">
         <v>122</v>
       </c>
@@ -2954,7 +2968,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2">
       <c r="A70">
         <v>123</v>
       </c>
@@ -2962,7 +2976,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2">
       <c r="A71">
         <v>124</v>
       </c>
@@ -2970,7 +2984,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2">
       <c r="A72">
         <v>125</v>
       </c>
@@ -2978,7 +2992,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2">
       <c r="A73">
         <v>126</v>
       </c>
@@ -2986,7 +3000,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2">
       <c r="A74">
         <v>127</v>
       </c>
@@ -2994,7 +3008,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2">
       <c r="A75">
         <v>128</v>
       </c>
@@ -3002,7 +3016,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2">
       <c r="A76">
         <v>129</v>
       </c>
@@ -3010,7 +3024,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:2">
       <c r="A77">
         <v>130</v>
       </c>
@@ -3018,7 +3032,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:2">
       <c r="A78">
         <v>132</v>
       </c>
@@ -3026,7 +3040,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:2">
       <c r="A79">
         <v>134</v>
       </c>
@@ -3034,7 +3048,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:2">
       <c r="A80">
         <v>135</v>
       </c>
@@ -3042,7 +3056,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2">
       <c r="A81">
         <v>136</v>
       </c>
@@ -3050,7 +3064,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:2">
       <c r="A82">
         <v>137</v>
       </c>
@@ -3058,7 +3072,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:2">
       <c r="A83">
         <v>138</v>
       </c>
@@ -3066,7 +3080,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:2">
       <c r="A84">
         <v>139</v>
       </c>
@@ -3074,7 +3088,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:2">
       <c r="A85">
         <v>140</v>
       </c>
@@ -3082,7 +3096,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:2">
       <c r="A86">
         <v>141</v>
       </c>
@@ -3090,7 +3104,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:2">
       <c r="A87">
         <v>142</v>
       </c>
@@ -3098,7 +3112,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:2">
       <c r="A88">
         <v>143</v>
       </c>
@@ -3106,7 +3120,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:2">
       <c r="A89">
         <v>144</v>
       </c>
@@ -3114,7 +3128,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:2">
       <c r="A90">
         <v>145</v>
       </c>
@@ -3122,7 +3136,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:2">
       <c r="A91">
         <v>146</v>
       </c>
@@ -3130,7 +3144,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:2">
       <c r="A92">
         <v>147</v>
       </c>
@@ -3138,7 +3152,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:2">
       <c r="A93">
         <v>148</v>
       </c>
@@ -3146,7 +3160,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:2">
       <c r="A94">
         <v>151</v>
       </c>
@@ -3154,7 +3168,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:2">
       <c r="A95">
         <v>152</v>
       </c>
@@ -3162,7 +3176,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:2">
       <c r="A96">
         <v>153</v>
       </c>
@@ -3170,7 +3184,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:2">
       <c r="A97">
         <v>154</v>
       </c>
@@ -3178,7 +3192,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:2">
       <c r="A98">
         <v>155</v>
       </c>
@@ -3186,7 +3200,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:2">
       <c r="A99">
         <v>156</v>
       </c>
@@ -3194,7 +3208,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:2">
       <c r="A100">
         <v>157</v>
       </c>
@@ -3202,7 +3216,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:2">
       <c r="A101">
         <v>158</v>
       </c>
@@ -3210,7 +3224,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:2">
       <c r="A102">
         <v>159</v>
       </c>
@@ -3218,7 +3232,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:2">
       <c r="A103">
         <v>165</v>
       </c>
@@ -3226,7 +3240,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:2">
       <c r="A104">
         <v>166</v>
       </c>
@@ -3234,7 +3248,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:2">
       <c r="A105">
         <v>167</v>
       </c>
@@ -3242,7 +3256,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:2">
       <c r="A106">
         <v>168</v>
       </c>

</xml_diff>